<commit_message>
Facturation + Gestion des véhicules amélioré
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -100,18 +100,19 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">échappement - amortisseurs - freins - vidanges - pneumatiques - mécanique - </t>
+      <t xml:space="preserve">Echappement - Amortisseurs - Freins - Vidanges - Pneumatiques - Mécanique générale
+</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FFC00000"/>
         <rFont val="Cambria"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
-      <t>di@gnostic - climatisation</t>
+      <t>Di@gnostic &amp; Climatisation</t>
     </r>
   </si>
 </sst>
@@ -119,7 +120,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,7 +148,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
@@ -152,8 +156,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="16"/>
+      <color rgb="FFC00000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
       <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
@@ -167,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -176,26 +188,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -204,7 +216,7 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -212,17 +224,17 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -232,7 +244,7 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -240,12 +252,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -254,101 +266,102 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -361,150 +374,157 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,390 +829,412 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="51" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="54" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="50" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="55"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="6">
         <v>63400</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="54"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
-      <c r="H3" s="55"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="H3" s="50"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="58"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="61" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="63"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="64" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="65"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="F8" s="57"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="32">
+      <c r="G10" s="53"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="58"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <v>300000</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="H13" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-    </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="s">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="18"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="E29" s="28" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
+      <c r="F29" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="24"/>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="25"/>
-      <c r="C30" s="4"/>
-      <c r="E30" s="28" t="s">
+      <c r="G29" s="32"/>
+      <c r="H29" s="19">
+        <f>SUM(H14:H28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="F30" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="24"/>
-    </row>
-    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E31" s="28" t="s">
+      <c r="G30" s="32"/>
+      <c r="H30" s="28"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="24"/>
-    </row>
-    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E32" s="28" t="s">
+      <c r="G31" s="32"/>
+      <c r="H31" s="28"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="24"/>
-    </row>
-    <row r="33" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E33" s="28" t="s">
+      <c r="G32" s="32"/>
+      <c r="H32" s="28"/>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="24"/>
-    </row>
-    <row r="34" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E34" s="28" t="s">
+      <c r="G33" s="32"/>
+      <c r="H33" s="28"/>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="28" t="s">
+      <c r="G34" s="32"/>
+      <c r="H34" s="28"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="49" t="s">
+      <c r="G35" s="32"/>
+      <c r="H35" s="28">
+        <f>SUM(H29:H34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="48">
+      <c r="G36" s="30">
         <v>0.2</v>
       </c>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="28" t="s">
+      <c r="H36" s="28">
+        <f>G36*H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="29"/>
-      <c r="G37" s="24"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="28">
+        <f>SUM(H35:H36)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="E37:F37"/>
+  <mergeCells count="37">
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="E2:H4"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B3:C3"/>
@@ -1200,10 +1242,33 @@
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.61458333333333337" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.13541666666666666" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0">
     <oddFooter>&amp;C&amp;"-,Gras"&amp;9LEPAIX AUTOMABILE&amp;"-,Normal" S.A.R.L. au capital de 45 735€ - R.C. 326 737 426 - N° T.V.A. Intracommunautaire FR 3326737426 00055</oddFooter>
   </headerFooter>

</xml_diff>